<commit_message>
Add the obstacle spawn system which is responsible for spawning the obstacles and the cleanup system, which is responsible for removing the obstacles that we passed.
In addition, clean up some unused loggers and log messages.
</commit_message>
<xml_diff>
--- a/GameState_Template.xlsx
+++ b/GameState_Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t xml:space="preserve">                         COMPONENT
 ENTITY</t>
@@ -95,6 +95,33 @@
   </si>
   <si>
     <t>Logic for chaning bounds based on position</t>
+  </si>
+  <si>
+    <t>WorldWrapSystem</t>
+  </si>
+  <si>
+    <t>Logic for containing the player into the world's bounds</t>
+  </si>
+  <si>
+    <t>WorldWrap</t>
+  </si>
+  <si>
+    <t>ObstacleSpawnSystem</t>
+  </si>
+  <si>
+    <t>Logic for spawning obstacles</t>
+  </si>
+  <si>
+    <t>Obstacle</t>
+  </si>
+  <si>
+    <t>CleanupSystem</t>
+  </si>
+  <si>
+    <t>Logic for cleaning up unused entities (that fell off-screen)</t>
+  </si>
+  <si>
+    <t>CleanupComponent</t>
   </si>
 </sst>
 </file>
@@ -592,7 +619,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -601,7 +628,8 @@
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="6" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
@@ -698,7 +726,12 @@
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="13"/>
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -708,7 +741,12 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -718,7 +756,12 @@
       <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -814,8 +857,12 @@
       <c r="E20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -911,13 +958,15 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+    <row r="27" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -925,7 +974,9 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -937,14 +988,16 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+    <row r="29" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1043,7 +1096,9 @@
       <c r="E39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -1058,19 +1113,21 @@
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+    <row r="41" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>

</xml_diff>

<commit_message>
Add collistion system to detect collision with osbtacles. Add the Hud System to render the HUD
</commit_message>
<xml_diff>
--- a/GameState_Template.xlsx
+++ b/GameState_Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t xml:space="preserve">                         COMPONENT
 ENTITY</t>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t>CleanupComponent</t>
+  </si>
+  <si>
+    <t>CollisionSystem</t>
+  </si>
+  <si>
+    <t>Logic for handling collisions</t>
+  </si>
+  <si>
+    <t>CollusionSystem</t>
+  </si>
+  <si>
+    <t>ObstacleComponent</t>
+  </si>
+  <si>
+    <t>HudRenderSystem</t>
+  </si>
+  <si>
+    <t>Logic for rendering HUD</t>
+  </si>
+  <si>
+    <t>HudRenderingSystem</t>
   </si>
 </sst>
 </file>
@@ -618,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -630,6 +651,7 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
@@ -771,7 +793,12 @@
       <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="13"/>
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -781,7 +808,12 @@
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="13"/>
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -863,7 +895,9 @@
       <c r="G20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1003,21 +1037,25 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="1"/>
+    <row r="30" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="12"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1099,7 +1137,9 @@
       <c r="F39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -1129,7 +1169,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="12"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>

</xml_diff>

<commit_message>
Add the render system to attach texture to our objects. Add the background.
</commit_message>
<xml_diff>
--- a/GameState_Template.xlsx
+++ b/GameState_Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t xml:space="preserve">                         COMPONENT
 ENTITY</t>
@@ -143,6 +143,30 @@
   </si>
   <si>
     <t>HudRenderingSystem</t>
+  </si>
+  <si>
+    <t>ScoreSystem</t>
+  </si>
+  <si>
+    <t>Logic for scoring</t>
+  </si>
+  <si>
+    <t>RenderSystem</t>
+  </si>
+  <si>
+    <t>Logic for rendering textures</t>
+  </si>
+  <si>
+    <t>Texture</t>
+  </si>
+  <si>
+    <t>TextureComponent</t>
+  </si>
+  <si>
+    <t>DimensionComponent</t>
+  </si>
+  <si>
+    <t>Dimension</t>
   </si>
 </sst>
 </file>
@@ -295,7 +319,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
@@ -317,6 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -637,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,179 +686,189 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
+      <c r="A14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -863,14 +898,14 @@
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:11" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -899,8 +934,12 @@
         <v>34</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="J20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1067,33 +1106,37 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" s="8" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+    <row r="32" spans="1:11" s="13" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" s="8" customFormat="1" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" s="8" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1107,6 +1150,16 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1115,80 +1168,87 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K38" s="11"/>
     </row>
-    <row r="39" spans="1:11" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="11"/>
+    </row>
+    <row r="40" spans="1:11" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="H40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
     </row>
     <row r="41" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
-      <c r="D41" s="1"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="12"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+    <row r="42" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="B17:I17"/>

</xml_diff>

<commit_message>
Fix the texture positioning and world wrapping related bugs.
</commit_message>
<xml_diff>
--- a/GameState_Template.xlsx
+++ b/GameState_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21060"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t xml:space="preserve">                         COMPONENT
 ENTITY</t>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Dimension</t>
+  </si>
+  <si>
+    <t>Background</t>
   </si>
 </sst>
 </file>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -679,6 +682,7 @@
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1235,16 +1239,18 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
+      <c r="I43" s="12"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>

</xml_diff>